<commit_message>
new plot constant learning rate
</commit_message>
<xml_diff>
--- a/graphs/iterations vs error graphs.xlsx
+++ b/graphs/iterations vs error graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\Desktop\COMP551\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\Desktop\COMP551\project1\project1\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514E45A5-E27D-42B7-94B0-EADFDE3945FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC569602-338E-485D-9B90-1F1CC1DF1560}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{798E7619-3329-46AF-8A99-A02B20450A3E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>wine dataset</t>
   </si>
@@ -638,16 +638,540 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8702014868110645E-2"/>
+          <c:y val="3.5772357723577237E-2"/>
+          <c:w val="0.91586761035947528"/>
+          <c:h val="0.81982664362076696"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>0.002</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$4:$R$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.41777233542319703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6540-4BA3-830D-DF31A31B2F81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0.005</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$4:$S$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.46529388714733499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42341496865203698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31211598746081498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27958268025078298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26641653605015603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27016457680250699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.272664576802507</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.27453957680250701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6540-4BA3-830D-DF31A31B2F81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0.01</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$4:$T$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.46529388714733499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46404388714733502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39903800940438799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34526645768024999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33776057993730402</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32775078369905902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.322746865203761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.31961598746081499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31398315047021902</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31085423197492101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.31022923197492103</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30522727272727201</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.30334247648902801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.30208659874608101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.30333268025078303</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.300199843260188</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29894788401253902</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.29957484326018802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.300199843260188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6540-4BA3-830D-DF31A31B2F81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>0.02</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -735,66 +1259,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$4:$N$22</c:f>
+              <c:f>Sheet1!$U$4:$U$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.41468652037617498</c:v>
+                  <c:v>0.46529388714733499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41718652037617499</c:v>
+                  <c:v>0.46466888714733501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37093652037617503</c:v>
+                  <c:v>0.40653996865203701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33714733542319703</c:v>
+                  <c:v>0.34776449843260099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32965321316614399</c:v>
+                  <c:v>0.33526057993730402</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32276645768024997</c:v>
+                  <c:v>0.32837578369905901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31776449843260102</c:v>
+                  <c:v>0.32399882445140998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31525862068965499</c:v>
+                  <c:v>0.32337186520376099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31462774294670798</c:v>
+                  <c:v>0.32023902821316602</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.312760579937304</c:v>
+                  <c:v>0.31648510971786797</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30837970219435701</c:v>
+                  <c:v>0.31648510971786797</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.30525470219435702</c:v>
+                  <c:v>0.31460423197492099</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.30524686520376099</c:v>
+                  <c:v>0.31210227272727198</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.30024490595611197</c:v>
+                  <c:v>0.31147727272727199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.298994905956112</c:v>
+                  <c:v>0.30834443573667702</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30024490595611197</c:v>
+                  <c:v>0.30771943573667698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29899098746081498</c:v>
+                  <c:v>0.302082680250783</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30024098746081501</c:v>
+                  <c:v>0.30082876175548501</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29961598746081503</c:v>
+                  <c:v>0.30020180250783601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,7 +1330,179 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>0.05</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$4:$V$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.46529388714733499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46529388714733499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.407164968652037</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34463166144200602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33400862068965498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32962578369905898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32399882445140998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.322746865203761</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32023902821316602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31961010971786802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.31710815047021901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31460619122257</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.313979231974921</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.310850313479623</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.30771943573667698</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30583855799373</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.30145768025078301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.30083072100313402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.30020180250783701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6540-4BA3-830D-DF31A31B2F81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -864,6 +1560,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44924115544830762"/>
+              <c:y val="0.89661925126492059"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -939,7 +1643,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.42000000000000004"/>
-          <c:min val="0.29500000000000004"/>
+          <c:min val="0.26"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -983,6 +1687,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3416840879914026E-2"/>
+              <c:y val="0.30169311574558116"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1061,6 +1773,50 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27578077181991506"/>
+          <c:y val="0.94755208046546624"/>
+          <c:w val="0.30120949240380407"/>
+          <c:h val="3.5742906046994434E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1078,9 +1834,8 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -2257,20 +3012,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>526255</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>204788</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>564355</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="3" name="Chart 2" descr="Learning rates:&#10;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96855BD1-E534-4BDA-B1F5-7E4115928D8C}"/>
@@ -2591,20 +3346,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657B8190-B84B-42E8-8E53-7BD518C7F5A3}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="R2">
+        <v>2E-3</v>
+      </c>
+      <c r="S2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="T2">
+        <v>0.01</v>
+      </c>
+      <c r="U2">
+        <v>0.02</v>
+      </c>
+      <c r="V2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2614,19 +3386,40 @@
       <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
+      <c r="S3" t="s">
         <v>2</v>
       </c>
+      <c r="T3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="L4">
         <v>10</v>
       </c>
-      <c r="N4">
-        <v>0.41468652037617498</v>
+      <c r="R4">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S4">
+        <v>0.46529388714733499</v>
+      </c>
+      <c r="T4">
+        <v>0.46529388714733499</v>
+      </c>
+      <c r="U4">
+        <v>0.46529388714733499</v>
+      </c>
+      <c r="V4">
+        <v>0.46529388714733499</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2636,11 +3429,23 @@
       <c r="L5">
         <v>20</v>
       </c>
-      <c r="N5">
-        <v>0.41718652037617499</v>
+      <c r="R5">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S5">
+        <v>0.42341496865203698</v>
+      </c>
+      <c r="T5">
+        <v>0.46404388714733502</v>
+      </c>
+      <c r="U5">
+        <v>0.46466888714733501</v>
+      </c>
+      <c r="V5">
+        <v>0.46529388714733499</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2650,11 +3455,23 @@
       <c r="L6">
         <v>30</v>
       </c>
-      <c r="N6">
-        <v>0.37093652037617503</v>
+      <c r="R6">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S6">
+        <v>0.31211598746081498</v>
+      </c>
+      <c r="T6">
+        <v>0.39903800940438799</v>
+      </c>
+      <c r="U6">
+        <v>0.40653996865203701</v>
+      </c>
+      <c r="V6">
+        <v>0.407164968652037</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2664,11 +3481,23 @@
       <c r="L7">
         <v>40</v>
       </c>
-      <c r="N7">
-        <v>0.33714733542319703</v>
+      <c r="R7">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S7">
+        <v>0.27958268025078298</v>
+      </c>
+      <c r="T7">
+        <v>0.34526645768024999</v>
+      </c>
+      <c r="U7">
+        <v>0.34776449843260099</v>
+      </c>
+      <c r="V7">
+        <v>0.34463166144200602</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2678,11 +3507,23 @@
       <c r="L8">
         <v>50</v>
       </c>
-      <c r="N8">
-        <v>0.32965321316614399</v>
+      <c r="R8">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S8">
+        <v>0.26641653605015603</v>
+      </c>
+      <c r="T8">
+        <v>0.33776057993730402</v>
+      </c>
+      <c r="U8">
+        <v>0.33526057993730402</v>
+      </c>
+      <c r="V8">
+        <v>0.33400862068965498</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2692,11 +3533,23 @@
       <c r="L9">
         <v>60</v>
       </c>
-      <c r="N9">
-        <v>0.32276645768024997</v>
+      <c r="R9">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S9">
+        <v>0.27016457680250699</v>
+      </c>
+      <c r="T9">
+        <v>0.32775078369905902</v>
+      </c>
+      <c r="U9">
+        <v>0.32837578369905901</v>
+      </c>
+      <c r="V9">
+        <v>0.32962578369905898</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2706,11 +3559,23 @@
       <c r="L10">
         <v>70</v>
       </c>
-      <c r="N10">
-        <v>0.31776449843260102</v>
+      <c r="R10">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S10">
+        <v>0.272664576802507</v>
+      </c>
+      <c r="T10">
+        <v>0.322746865203761</v>
+      </c>
+      <c r="U10">
+        <v>0.32399882445140998</v>
+      </c>
+      <c r="V10">
+        <v>0.32399882445140998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2720,11 +3585,23 @@
       <c r="L11">
         <v>80</v>
       </c>
-      <c r="N11">
-        <v>0.31525862068965499</v>
+      <c r="R11">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S11">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T11">
+        <v>0.31961598746081499</v>
+      </c>
+      <c r="U11">
+        <v>0.32337186520376099</v>
+      </c>
+      <c r="V11">
+        <v>0.322746865203761</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2734,11 +3611,23 @@
       <c r="L12">
         <v>90</v>
       </c>
-      <c r="N12">
-        <v>0.31462774294670798</v>
+      <c r="R12">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S12">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T12">
+        <v>0.31398315047021902</v>
+      </c>
+      <c r="U12">
+        <v>0.32023902821316602</v>
+      </c>
+      <c r="V12">
+        <v>0.32023902821316602</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2748,11 +3637,23 @@
       <c r="L13">
         <v>100</v>
       </c>
-      <c r="N13">
-        <v>0.312760579937304</v>
+      <c r="R13">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S13">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T13">
+        <v>0.31085423197492101</v>
+      </c>
+      <c r="U13">
+        <v>0.31648510971786797</v>
+      </c>
+      <c r="V13">
+        <v>0.31961010971786802</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2762,11 +3663,23 @@
       <c r="L14">
         <v>150</v>
       </c>
-      <c r="N14">
-        <v>0.30837970219435701</v>
+      <c r="R14">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S14">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T14">
+        <v>0.31022923197492103</v>
+      </c>
+      <c r="U14">
+        <v>0.31648510971786797</v>
+      </c>
+      <c r="V14">
+        <v>0.31710815047021901</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2776,11 +3689,23 @@
       <c r="L15">
         <v>200</v>
       </c>
-      <c r="N15">
-        <v>0.30525470219435702</v>
+      <c r="R15">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S15">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T15">
+        <v>0.30522727272727201</v>
+      </c>
+      <c r="U15">
+        <v>0.31460423197492099</v>
+      </c>
+      <c r="V15">
+        <v>0.31460619122257</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2790,11 +3715,23 @@
       <c r="L16">
         <v>250</v>
       </c>
-      <c r="N16">
-        <v>0.30524686520376099</v>
+      <c r="R16">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S16">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T16">
+        <v>0.30334247648902801</v>
+      </c>
+      <c r="U16">
+        <v>0.31210227272727198</v>
+      </c>
+      <c r="V16">
+        <v>0.313979231974921</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2804,11 +3741,23 @@
       <c r="L17">
         <v>300</v>
       </c>
-      <c r="N17">
-        <v>0.30024490595611197</v>
+      <c r="R17">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S17">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T17">
+        <v>0.30208659874608101</v>
+      </c>
+      <c r="U17">
+        <v>0.31147727272727199</v>
+      </c>
+      <c r="V17">
+        <v>0.310850313479623</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2818,11 +3767,23 @@
       <c r="L18">
         <v>350</v>
       </c>
-      <c r="N18">
-        <v>0.298994905956112</v>
+      <c r="R18">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S18">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T18">
+        <v>0.30333268025078303</v>
+      </c>
+      <c r="U18">
+        <v>0.30834443573667702</v>
+      </c>
+      <c r="V18">
+        <v>0.30771943573667698</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2832,11 +3793,23 @@
       <c r="L19">
         <v>400</v>
       </c>
-      <c r="N19">
-        <v>0.30024490595611197</v>
+      <c r="R19">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S19">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T19">
+        <v>0.300199843260188</v>
+      </c>
+      <c r="U19">
+        <v>0.30771943573667698</v>
+      </c>
+      <c r="V19">
+        <v>0.30583855799373</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2846,11 +3819,23 @@
       <c r="L20">
         <v>500</v>
       </c>
-      <c r="N20">
-        <v>0.29899098746081498</v>
+      <c r="R20">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S20">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T20">
+        <v>0.29894788401253902</v>
+      </c>
+      <c r="U20">
+        <v>0.302082680250783</v>
+      </c>
+      <c r="V20">
+        <v>0.30145768025078301</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2860,11 +3845,23 @@
       <c r="L21">
         <v>600</v>
       </c>
-      <c r="N21">
-        <v>0.30024098746081501</v>
+      <c r="R21">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S21">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T21">
+        <v>0.29957484326018802</v>
+      </c>
+      <c r="U21">
+        <v>0.30082876175548501</v>
+      </c>
+      <c r="V21">
+        <v>0.30083072100313402</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2874,11 +3871,23 @@
       <c r="L22">
         <v>700</v>
       </c>
-      <c r="N22">
-        <v>0.29961598746081503</v>
+      <c r="R22">
+        <v>0.41777233542319703</v>
+      </c>
+      <c r="S22">
+        <v>0.27453957680250701</v>
+      </c>
+      <c r="T22">
+        <v>0.300199843260188</v>
+      </c>
+      <c r="U22">
+        <v>0.30020180250783601</v>
+      </c>
+      <c r="V22">
+        <v>0.30020180250783701</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2886,7 +3895,7 @@
         <v>0.27767241379310298</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2894,7 +3903,7 @@
         <v>0.27767241379310298</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>30</v>
       </c>
@@ -2902,7 +3911,7 @@
         <v>0.27829741379310302</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>40</v>
       </c>
@@ -2910,7 +3919,7 @@
         <v>0.27829545454545401</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>50</v>
       </c>
@@ -2918,7 +3927,7 @@
         <v>0.27829545454545401</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>75</v>
       </c>

</xml_diff>